<commit_message>
Ship header part 1
</commit_message>
<xml_diff>
--- a/DataSource/excel/shipStyle.xlsx
+++ b/DataSource/excel/shipStyle.xlsx
@@ -206,9 +206,6 @@
     <t>2_42_370;1_148_340;1_275_340;3_97_266;3_177_266;9_257_266;4_337_266;5_257_202;6_337_202;7_97_202;7_177_202;8_417_202;8_417_266;8_497_266</t>
   </si>
   <si>
-    <t>0;2;2;0;0;0;0;0;0;0;1;1;2;2</t>
-  </si>
-  <si>
     <t>小型三角帆船</t>
   </si>
   <si>
@@ -273,6 +270,9 @@
   </si>
   <si>
     <t>duration</t>
+  </si>
+  <si>
+    <t>0;2;2;0;-1;0;0;0;0;0;1;1;2;2</t>
   </si>
 </sst>
 </file>
@@ -724,8 +724,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N7" sqref="H7:N19"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -734,7 +734,7 @@
     <col min="3" max="3" width="21.1640625" customWidth="1"/>
     <col min="4" max="4" width="13.33203125" customWidth="1"/>
     <col min="6" max="6" width="125.33203125" customWidth="1"/>
-    <col min="7" max="7" width="18.83203125" customWidth="1"/>
+    <col min="7" max="7" width="31" customWidth="1"/>
     <col min="11" max="11" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12.5" bestFit="1" customWidth="1"/>
@@ -745,10 +745,10 @@
         <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D1" t="s">
         <v>11</v>
@@ -763,25 +763,25 @@
         <v>13</v>
       </c>
       <c r="H1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
@@ -1009,7 +1009,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7" s="1">
         <v>2</v>
@@ -1024,7 +1024,7 @@
         <v>16</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="H7">
         <v>25</v>
@@ -1053,7 +1053,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8" s="1">
         <v>13</v>
@@ -1097,7 +1097,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C9" s="1">
         <v>24</v>
@@ -1141,7 +1141,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C10" s="1">
         <v>29</v>
@@ -1185,7 +1185,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C11" s="1">
         <v>30</v>
@@ -1229,7 +1229,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C12" s="1">
         <v>31</v>
@@ -1273,7 +1273,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C13" s="1">
         <v>3</v>
@@ -1317,7 +1317,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C14" s="1">
         <v>4</v>
@@ -1361,7 +1361,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C15" s="1">
         <v>5</v>
@@ -1405,7 +1405,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C16" s="1">
         <v>14</v>
@@ -1449,7 +1449,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C17" s="1">
         <v>15</v>
@@ -1493,7 +1493,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C18" s="1">
         <v>16</v>
@@ -1537,7 +1537,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C19" s="1">
         <v>17</v>

</xml_diff>